<commit_message>
stream read from txt & excel
</commit_message>
<xml_diff>
--- a/outputFiles/WriteLines.xlsx
+++ b/outputFiles/WriteLines.xlsx
@@ -2,13 +2,40 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mySheet" sheetId="1" r:id="Rfd04c54d3d794293"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="mySheet" sheetId="1" r:id="R5ac3fa53e6a14aaa"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row>
+      <x:c t="str">
+        <x:v>First Header</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Second Header</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>Third Header</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>First line</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Second line</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>Third line</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
 </x:worksheet>
 </file>
</xml_diff>